<commit_message>
fix: use ZodError type in report-templates API
Import and use ZodError instead of checking error.name for
more reliable validation error handling.
</commit_message>
<xml_diff>
--- a/demo-khach-hang.xlsx
+++ b/demo-khach-hang.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11214"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC730CEA-8263-1B41-9F82-DCEE827E9DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="KhachHang" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="HuongDan" state="visible" r:id="rId5"/>
+    <sheet name="KhachHang" sheetId="1" r:id="rId1"/>
+    <sheet name="HuongDan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>ho_ten</t>
   </si>
@@ -38,9 +42,6 @@
     <t>0901234567</t>
   </si>
   <si>
-    <t>CN Hà Nội</t>
-  </si>
-  <si>
     <t>Đống Đa, Hà Nội</t>
   </si>
   <si>
@@ -71,9 +72,6 @@
     <t>0923456789</t>
   </si>
   <si>
-    <t>CN HCM</t>
-  </si>
-  <si>
     <t>Quận 1, TP.HCM</t>
   </si>
   <si>
@@ -104,9 +102,6 @@
     <t>0945678901</t>
   </si>
   <si>
-    <t>CN Đà Nẵng</t>
-  </si>
-  <si>
     <t>Hải Châu, Đà Nẵng</t>
   </si>
   <si>
@@ -195,30 +190,53 @@
   </si>
   <si>
     <t>- Tên chi nhánh phải chính xác (phân biệt hoa thường)</t>
+  </si>
+  <si>
+    <t>Càng Long</t>
+  </si>
+  <si>
+    <t>Cầu Kè</t>
+  </si>
+  <si>
+    <t>Tiểu Cần</t>
+  </si>
+  <si>
+    <t>Châu Thành</t>
+  </si>
+  <si>
+    <t>Trà Cú</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -251,10 +269,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,9 +611,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -605,7 +628,7 @@
     <col min="6" max="6" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -633,266 +656,271 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -900,6 +928,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>